<commit_message>
radar plot early draft
</commit_message>
<xml_diff>
--- a/president_bios.xlsx
+++ b/president_bios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbcme\OneDrive\Documentos\GitHub\data-vis-nova\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC2FCB-181E-4C3A-97D6-8F0C12F566CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD502694-7B79-4E8D-A0CD-C93EA00FAC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{D2D1368C-2394-42C4-B1D9-93BBF7FE5F04}"/>
+    <workbookView xWindow="8595" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{D2D1368C-2394-42C4-B1D9-93BBF7FE5F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -1044,13 +1044,13 @@
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>81268924</v>
+        <v>74216154</v>
       </c>
       <c r="G12" s="1">
-        <v>51.3</v>
+        <v>46.9</v>
       </c>
       <c r="H12" s="1">
-        <v>306</v>
+        <v>232</v>
       </c>
       <c r="I12" s="1">
         <v>25</v>
@@ -1091,13 +1091,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>74216154</v>
+        <v>81268924</v>
       </c>
       <c r="G13" s="1">
-        <v>46.9</v>
+        <v>51.3</v>
       </c>
       <c r="H13" s="1">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="I13" s="1">
         <v>25</v>

</xml_diff>